<commit_message>
1st draft of code complete!
</commit_message>
<xml_diff>
--- a/MAE 159/Other data/159 Digitized Plots.xlsx
+++ b/MAE 159/Other data/159 Digitized Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy Slagle\Documents\MAE136-MAE158-MAE159_Aircraft_Design_and_Analysis_Course_Series\MAE 159\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3223F2-9121-489D-A29B-BF452203D264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60630B69-B0AD-4CD6-B05B-F003EB9EC074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="6495" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5970" yWindow="2430" windowWidth="28800" windowHeight="15435" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 1a" sheetId="6" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="Figure 3" sheetId="3" r:id="rId4"/>
     <sheet name="Figure 4" sheetId="4" r:id="rId5"/>
     <sheet name="Figure 5" sheetId="5" r:id="rId6"/>
-    <sheet name="Shevel_3" sheetId="7" r:id="rId7"/>
-    <sheet name="Shevel_1" sheetId="8" r:id="rId8"/>
-    <sheet name="Shevel_2" sheetId="9" r:id="rId9"/>
-    <sheet name="JT9D_Thrust" sheetId="10" r:id="rId10"/>
+    <sheet name="Figure 6" sheetId="11" r:id="rId7"/>
+    <sheet name="Shevel_3" sheetId="7" r:id="rId8"/>
+    <sheet name="Shevel_1" sheetId="8" r:id="rId9"/>
+    <sheet name="Shevel_2" sheetId="9" r:id="rId10"/>
+    <sheet name="JT9D_Thrust" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Range</t>
   </si>
@@ -202,6 +203,18 @@
   </si>
   <si>
     <t>25, T</t>
+  </si>
+  <si>
+    <t>to, cd</t>
+  </si>
+  <si>
+    <t>to, cl</t>
+  </si>
+  <si>
+    <t>l, cd</t>
+  </si>
+  <si>
+    <t>l, cl</t>
   </si>
 </sst>
 </file>
@@ -18827,6 +18840,669 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596094CB-5E7C-4458-92EE-C2DA16EDDB8D}">
+  <dimension ref="A1:B81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.0465455966455597</v>
+      </c>
+      <c r="B2">
+        <v>1.3971791027042799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.0543895497041298</v>
+      </c>
+      <c r="B3">
+        <v>1.3907254301576699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.0959568161710198</v>
+      </c>
+      <c r="B4">
+        <v>1.38546817295806</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.1513567102403002</v>
+      </c>
+      <c r="B5">
+        <v>1.37970492324917</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.1887808578635397</v>
+      </c>
+      <c r="B6">
+        <v>1.37440870669709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.2253637958448804</v>
+      </c>
+      <c r="B7">
+        <v>1.3695735934192801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.2620241853533498</v>
+      </c>
+      <c r="B8">
+        <v>1.36488312691928</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.2987878435646696</v>
+      </c>
+      <c r="B9">
+        <v>1.3603855227897099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.3355773189516897</v>
+      </c>
+      <c r="B10">
+        <v>1.3559361342527501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.3722358643761901</v>
+      </c>
+      <c r="B11">
+        <v>1.35124222378185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.3967685433905999</v>
+      </c>
+      <c r="B12">
+        <v>1.3476782080568099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.44748177486332</v>
+      </c>
+      <c r="B13">
+        <v>1.3436277090033399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.4872360147985999</v>
+      </c>
+      <c r="B14">
+        <v>1.33841565308246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.51990826535451</v>
+      </c>
+      <c r="B15">
+        <v>1.3344055375152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4.5578610503851396</v>
+      </c>
+      <c r="B16">
+        <v>1.33009659262123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.6066711592505696</v>
+      </c>
+      <c r="B17">
+        <v>1.3251890514898901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4.65440201237897</v>
+      </c>
+      <c r="B18">
+        <v>1.3203904134073601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4.70081742172954</v>
+      </c>
+      <c r="B19">
+        <v>1.3156290565734099</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4.7474290416155096</v>
+      </c>
+      <c r="B20">
+        <v>1.31123413824325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4.7939787002797702</v>
+      </c>
+      <c r="B21">
+        <v>1.3067235024908499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4.8408484919228396</v>
+      </c>
+      <c r="B22">
+        <v>1.3028107400867499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4.9003374178526702</v>
+      </c>
+      <c r="B23">
+        <v>1.29747002243305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4.9629700998502004</v>
+      </c>
+      <c r="B24">
+        <v>1.2938268365648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5.0157660634112498</v>
+      </c>
+      <c r="B25">
+        <v>1.2883199425843199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5.0783802662936699</v>
+      </c>
+      <c r="B26">
+        <v>1.2819716837888899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5.1661822485718503</v>
+      </c>
+      <c r="B27">
+        <v>1.27680846732852</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5.2223169844946096</v>
+      </c>
+      <c r="B28">
+        <v>1.2724901681905101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5.2862296847862797</v>
+      </c>
+      <c r="B29">
+        <v>1.26752284334673</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5.3654502752069897</v>
+      </c>
+      <c r="B30">
+        <v>1.26227214688423</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5.4471003205374497</v>
+      </c>
+      <c r="B31">
+        <v>1.2572120046486399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5.5240129141250698</v>
+      </c>
+      <c r="B32">
+        <v>1.2527101507699101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5.5626644533101999</v>
+      </c>
+      <c r="B33">
+        <v>1.24781920784962</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5.66157500174796</v>
+      </c>
+      <c r="B34">
+        <v>1.2452567175346401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5.7136494577803303</v>
+      </c>
+      <c r="B35">
+        <v>1.24108817140108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5.80422931213654</v>
+      </c>
+      <c r="B36">
+        <v>1.2365061819624199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5.8851306593714003</v>
+      </c>
+      <c r="B37">
+        <v>1.2321379763412601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5.9709103770998198</v>
+      </c>
+      <c r="B38">
+        <v>1.2277359327395401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6.0548488999138499</v>
+      </c>
+      <c r="B39">
+        <v>1.2235531441918299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6.1026027454165899</v>
+      </c>
+      <c r="B40">
+        <v>1.22024632703739</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6.1903470477674496</v>
+      </c>
+      <c r="B41">
+        <v>1.2169005627012399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6.2811164367025096</v>
+      </c>
+      <c r="B42">
+        <v>1.21267254389598</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6.3768077984723401</v>
+      </c>
+      <c r="B43">
+        <v>1.20849211788877</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6.4724681796313197</v>
+      </c>
+      <c r="B44">
+        <v>1.20425383317044</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>6.56813888766058</v>
+      </c>
+      <c r="B45">
+        <v>1.2000348346891501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6.67859241270917</v>
+      </c>
+      <c r="B46">
+        <v>1.19599017389903</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6.75531848279042</v>
+      </c>
+      <c r="B47">
+        <v>1.192968888</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>6.8605939178174697</v>
+      </c>
+      <c r="B48">
+        <v>1.18839831555637</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>6.9661374658907</v>
+      </c>
+      <c r="B49">
+        <v>1.1843284651728301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7.0683889178465797</v>
+      </c>
+      <c r="B50">
+        <v>1.1811446573258899</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>7.1964876956409398</v>
+      </c>
+      <c r="B51">
+        <v>1.1755858673430899</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>7.30212512435312</v>
+      </c>
+      <c r="B52">
+        <v>1.1716913463872101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>7.4077813291930896</v>
+      </c>
+      <c r="B53">
+        <v>1.1678318913168599</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>7.5134656982247501</v>
+      </c>
+      <c r="B54">
+        <v>1.1640250350748</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>7.6192627240231303</v>
+      </c>
+      <c r="B55">
+        <v>1.1604285741459399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>7.7250221975659503</v>
+      </c>
+      <c r="B56">
+        <v>1.1567619814460099</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>7.8308192233643403</v>
+      </c>
+      <c r="B57">
+        <v>1.1531655205171401</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>7.9331539007741103</v>
+      </c>
+      <c r="B58">
+        <v>1.14919923747657</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>8.0555112940146003</v>
+      </c>
+      <c r="B59">
+        <v>1.14561318052453</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>8.1469655154753902</v>
+      </c>
+      <c r="B60">
+        <v>1.1432789013753599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>8.2543546849219993</v>
+      </c>
+      <c r="B61">
+        <v>1.1394283956840101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>8.3602737555510203</v>
+      </c>
+      <c r="B62">
+        <v>1.1360598630111001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8.4663148710106704</v>
+      </c>
+      <c r="B63">
+        <v>1.1329192585941401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>8.5723090461508509</v>
+      </c>
+      <c r="B64">
+        <v>1.12969098946335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>8.6783877138660799</v>
+      </c>
+      <c r="B65">
+        <v>1.1266205168174599</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>8.7844476054535097</v>
+      </c>
+      <c r="B66">
+        <v>1.1235149782860301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>8.8904981089770594</v>
+      </c>
+      <c r="B67">
+        <v>1.12039190681184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>9.0007393562100599</v>
+      </c>
+      <c r="B68">
+        <v>1.1174748966169099</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>9.1016620698966708</v>
+      </c>
+      <c r="B69">
+        <v>1.11405840719547</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>9.2088937092089491</v>
+      </c>
+      <c r="B70">
+        <v>1.11147854890117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>9.3150287053075491</v>
+      </c>
+      <c r="B71">
+        <v>1.1085132739118699</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>9.4211918655978302</v>
+      </c>
+      <c r="B72">
+        <v>1.1056005977508601</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>9.5198648503826302</v>
+      </c>
+      <c r="B73">
+        <v>1.1029243296634199</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>9.6181313099348404</v>
+      </c>
+      <c r="B74">
+        <v>1.0991762088674</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>9.7301530483696297</v>
+      </c>
+      <c r="B75">
+        <v>1.0973568801696001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>9.8427682590989996</v>
+      </c>
+      <c r="B76">
+        <v>1.0949428689016301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>9.9425263092696596</v>
+      </c>
+      <c r="B77">
+        <v>1.09161919256142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>10.046718772450999</v>
+      </c>
+      <c r="B78">
+        <v>1.08894518958888</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>10.1839726437893</v>
+      </c>
+      <c r="B79">
+        <v>1.0853102852718099</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>10.290257848910199</v>
+      </c>
+      <c r="B80">
+        <v>1.0826255373667499</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>10.358126314235699</v>
+      </c>
+      <c r="B81">
+        <v>1.0813511345859499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C2F5D8-F9D3-4BC8-847A-B054563BDAE4}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -29333,7 +30009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB30471-B599-4A7E-AA66-1ED16431E92A}">
   <dimension ref="B1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
@@ -29400,7 +30076,7 @@
         <v>3037.7469948995199</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="C3:D66" si="0">C3*1000</f>
+        <f t="shared" ref="D3:D66" si="0">C3*1000</f>
         <v>3037746.9948995197</v>
       </c>
       <c r="F3">
@@ -30936,7 +31612,7 @@
         <v>8774.0720439686902</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="C67:D109" si="1">C67*1000</f>
+        <f t="shared" ref="D67:D109" si="1">C67*1000</f>
         <v>8774072.0439686906</v>
       </c>
       <c r="F67">
@@ -32457,6 +33133,1871 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0737387E-079F-42FD-BAAB-95AC0AD4E1E7}">
+  <dimension ref="A1:E137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.07094584094958E-2</v>
+      </c>
+      <c r="B2">
+        <v>0.57188338731219601</v>
+      </c>
+      <c r="D2">
+        <v>1.9183464122369199E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.54066713068513095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.0725883419809901E-2</v>
+      </c>
+      <c r="B3">
+        <v>0.58572154440674196</v>
+      </c>
+      <c r="D3">
+        <v>1.9209917484784299E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.47071712306292701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.07645110985089E-2</v>
+      </c>
+      <c r="B4">
+        <v>0.54869230259634405</v>
+      </c>
+      <c r="D4">
+        <v>1.9127280642343199E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.51905451755641396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.0864137133995901E-2</v>
+      </c>
+      <c r="B5">
+        <v>0.53573298158621696</v>
+      </c>
+      <c r="D5">
+        <v>1.9126019356786199E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.494499228201291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.09493233902948E-2</v>
+      </c>
+      <c r="B6">
+        <v>0.59731637678621996</v>
+      </c>
+      <c r="D6">
+        <v>1.9170099669969999E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.48260898414849202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.09303410426623E-2</v>
+      </c>
+      <c r="B7">
+        <v>0.51721498108253805</v>
+      </c>
+      <c r="D7">
+        <v>1.9164323628932101E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.52986421988957999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.1111503985502799E-2</v>
+      </c>
+      <c r="B8">
+        <v>0.49979129133249001</v>
+      </c>
+      <c r="D8">
+        <v>1.9424187262456798E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.44980686811584403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.1174385979658299E-2</v>
+      </c>
+      <c r="B9">
+        <v>0.61307324937464303</v>
+      </c>
+      <c r="D9">
+        <v>1.93531865877953E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.55406731950840604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.13743213204772E-2</v>
+      </c>
+      <c r="B10">
+        <v>0.48391689684526301</v>
+      </c>
+      <c r="D10">
+        <v>1.93260786505168E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.46197649500467902</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.14582211401403E-2</v>
+      </c>
+      <c r="B11">
+        <v>0.62483439512887695</v>
+      </c>
+      <c r="D11">
+        <v>1.9530416612944499E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.56881981262044401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.1601258717229199E-2</v>
+      </c>
+      <c r="B12">
+        <v>0.46864211966786901</v>
+      </c>
+      <c r="D12">
+        <v>1.96364935003428E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.433336095774424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.17404081846425E-2</v>
+      </c>
+      <c r="B13">
+        <v>0.63398341351911602</v>
+      </c>
+      <c r="D13">
+        <v>1.9746175138783E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.58222864583137701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.1869246538971499E-2</v>
+      </c>
+      <c r="B14">
+        <v>0.455803116675703</v>
+      </c>
+      <c r="D14">
+        <v>1.9812811981021701E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.42067198026594099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1.19436367299135E-2</v>
+      </c>
+      <c r="B15">
+        <v>0.64349218521275497</v>
+      </c>
+      <c r="D15">
+        <v>2.0006537979346001E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.59287339423752505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.21456278387877E-2</v>
+      </c>
+      <c r="B16">
+        <v>0.44404333482641201</v>
+      </c>
+      <c r="D16">
+        <v>2.0036143610311301E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.40699754268566102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.2206985923172599E-2</v>
+      </c>
+      <c r="B17">
+        <v>0.647589031428774</v>
+      </c>
+      <c r="D17">
+        <v>2.02868516043185E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.60527749398701503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1.2423716078391199E-2</v>
+      </c>
+      <c r="B18">
+        <v>0.43575574275287199</v>
+      </c>
+      <c r="D18">
+        <v>2.0283157839473001E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.394865253083378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1.2473425664838901E-2</v>
+      </c>
+      <c r="B19">
+        <v>0.65680446135468695</v>
+      </c>
+      <c r="D19">
+        <v>2.0538020599666799E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.38129569624825899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.2715444312776899E-2</v>
+      </c>
+      <c r="B20">
+        <v>0.42049848882054602</v>
+      </c>
+      <c r="D20">
+        <v>2.05604203255445E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.61652812072947605</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.27539870825554E-2</v>
+      </c>
+      <c r="B21">
+        <v>0.66315736266127301</v>
+      </c>
+      <c r="D21">
+        <v>2.0820689687290301E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.37040522312846302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.2991682666896801E-2</v>
+      </c>
+      <c r="B22">
+        <v>0.40990818145040198</v>
+      </c>
+      <c r="D22">
+        <v>2.0840573898197001E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.62621770446607605</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1.3034472293927801E-2</v>
+      </c>
+      <c r="B23">
+        <v>0.67013372712087305</v>
+      </c>
+      <c r="D23">
+        <v>2.1103228236268801E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.36058271929855001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1.3182057874802099E-2</v>
+      </c>
+      <c r="B24">
+        <v>0.67632072086573403</v>
+      </c>
+      <c r="D24">
+        <v>2.11209003463525E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.63449295049445298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1.3272130245506599E-2</v>
+      </c>
+      <c r="B25">
+        <v>0.39975533803943603</v>
+      </c>
+      <c r="D25">
+        <v>2.1385667999245499E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.351568408444766</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1.3417177496547601E-2</v>
+      </c>
+      <c r="B26">
+        <v>0.67780315182370698</v>
+      </c>
+      <c r="D26">
+        <v>2.1403676628547998E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.64016258269119997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.35546772618566E-2</v>
+      </c>
+      <c r="B27">
+        <v>0.38986356052585502</v>
+      </c>
+      <c r="D27">
+        <v>2.1668032496697201E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.34316986366802998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.36976468315983E-2</v>
+      </c>
+      <c r="B28">
+        <v>0.684909404440184</v>
+      </c>
+      <c r="D28">
+        <v>2.1681916634026601E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.64807044696044902</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1.3826365658182301E-2</v>
+      </c>
+      <c r="B29">
+        <v>0.38511083172299698</v>
+      </c>
+      <c r="D29">
+        <v>2.19205642936595E-2</v>
+      </c>
+      <c r="E29">
+        <v>0.33970285301722303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1.3978432517059099E-2</v>
+      </c>
+      <c r="B30">
+        <v>0.68942751526406199</v>
+      </c>
+      <c r="D30">
+        <v>2.1943087712043501E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.65612674675239602</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1.4119481287080401E-2</v>
+      </c>
+      <c r="B31">
+        <v>0.37245262916432598</v>
+      </c>
+      <c r="D31">
+        <v>2.2181385714591498E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.328200667952525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1.4259164693435701E-2</v>
+      </c>
+      <c r="B32">
+        <v>0.69438339728334197</v>
+      </c>
+      <c r="D32">
+        <v>2.2217516694700699E-2</v>
+      </c>
+      <c r="E32">
+        <v>0.66033935966107804</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.44018751851278E-2</v>
+      </c>
+      <c r="B33">
+        <v>0.363813550763743</v>
+      </c>
+      <c r="D33">
+        <v>2.2463684354708701E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.320340918493208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.45398357165731E-2</v>
+      </c>
+      <c r="B34">
+        <v>0.69983958924022505</v>
+      </c>
+      <c r="D34">
+        <v>2.2498093635931801E-2</v>
+      </c>
+      <c r="E34">
+        <v>0.66656525921427301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1.46926814756326E-2</v>
+      </c>
+      <c r="B35">
+        <v>0.35609895020802701</v>
+      </c>
+      <c r="D35">
+        <v>2.2754304539442501E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.314148895776447</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1.48206878473803E-2</v>
+      </c>
+      <c r="B36">
+        <v>0.70381409407420803</v>
+      </c>
+      <c r="D36">
+        <v>2.2795441852993301E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.67507788565260496</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1.4972168672474801E-2</v>
+      </c>
+      <c r="B37">
+        <v>0.34977928607702902</v>
+      </c>
+      <c r="D37">
+        <v>2.2736258453781098E-2</v>
+      </c>
+      <c r="E37">
+        <v>0.67103352500315905</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.51015940752836E-2</v>
+      </c>
+      <c r="B38">
+        <v>0.70734601704031097</v>
+      </c>
+      <c r="D38">
+        <v>2.3028133455940802E-2</v>
+      </c>
+      <c r="E38">
+        <v>0.305833709038766</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1.52487746335511E-2</v>
+      </c>
+      <c r="B39">
+        <v>0.34020543835093098</v>
+      </c>
+      <c r="D39">
+        <v>2.30594309781114E-2</v>
+      </c>
+      <c r="E39">
+        <v>0.67751612850785503</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1.53824038692329E-2</v>
+      </c>
+      <c r="B40">
+        <v>0.71166689029263297</v>
+      </c>
+      <c r="D40">
+        <v>2.33103191977704E-2</v>
+      </c>
+      <c r="E40">
+        <v>0.29889760869502402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1.55327347239491E-2</v>
+      </c>
+      <c r="B41">
+        <v>0.33484872500590201</v>
+      </c>
+      <c r="D41">
+        <v>2.33401603320307E-2</v>
+      </c>
+      <c r="E41">
+        <v>0.68249510175502504</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1.56633124491838E-2</v>
+      </c>
+      <c r="B42">
+        <v>0.71517957056882797</v>
+      </c>
+      <c r="D42">
+        <v>2.35924767150281E-2</v>
+      </c>
+      <c r="E42">
+        <v>0.29219242063017598</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1.5816760878454999E-2</v>
+      </c>
+      <c r="B43">
+        <v>0.32665212807500998</v>
+      </c>
+      <c r="D43">
+        <v>2.36240886765701E-2</v>
+      </c>
+      <c r="E43">
+        <v>0.68745796935585102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1.5962147974536E-2</v>
+      </c>
+      <c r="B44">
+        <v>0.71688941479556501</v>
+      </c>
+      <c r="D44">
+        <v>2.3874549558570199E-2</v>
+      </c>
+      <c r="E44">
+        <v>0.28617996940200802</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1.6113174854432401E-2</v>
+      </c>
+      <c r="B45">
+        <v>0.318281117279264</v>
+      </c>
+      <c r="D45">
+        <v>2.3901645853212802E-2</v>
+      </c>
+      <c r="E45">
+        <v>0.69223368158441501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1.6225066103799E-2</v>
+      </c>
+      <c r="B46">
+        <v>0.722724483748729</v>
+      </c>
+      <c r="D46">
+        <v>2.41565659529684E-2</v>
+      </c>
+      <c r="E46">
+        <v>0.28062934273162798</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1.6377784558278902E-2</v>
+      </c>
+      <c r="B47">
+        <v>0.31027699167142703</v>
+      </c>
+      <c r="D47">
+        <v>2.4177332181747099E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.69662188808108705</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1.65059252907491E-2</v>
+      </c>
+      <c r="B48">
+        <v>0.72664126051298805</v>
+      </c>
+      <c r="D48">
+        <v>2.4438589403509601E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.27502098799152402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1.6660190048561199E-2</v>
+      </c>
+      <c r="B49">
+        <v>0.301543074299156</v>
+      </c>
+      <c r="D49">
+        <v>2.4463303544283398E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.70056369651255401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1.6786773893484801E-2</v>
+      </c>
+      <c r="B50">
+        <v>0.73064462938183194</v>
+      </c>
+      <c r="D50">
+        <v>2.4720591685621799E-2</v>
+      </c>
+      <c r="E50">
+        <v>0.26958581746059102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1.6942287756607E-2</v>
+      </c>
+      <c r="B51">
+        <v>0.29532720034910598</v>
+      </c>
+      <c r="D51">
+        <v>2.4744099225946802E-2</v>
+      </c>
+      <c r="E51">
+        <v>0.70500002590432398</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1.7045703932092302E-2</v>
+      </c>
+      <c r="B52">
+        <v>0.73461631595870902</v>
+      </c>
+      <c r="D52">
+        <v>2.5028197182522902E-2</v>
+      </c>
+      <c r="E52">
+        <v>0.26392943684735598</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1.72245087791516E-2</v>
+      </c>
+      <c r="B53">
+        <v>0.28810245965674702</v>
+      </c>
+      <c r="D53">
+        <v>2.50249725251829E-2</v>
+      </c>
+      <c r="E53">
+        <v>0.70880134652913596</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1.7348643974459E-2</v>
+      </c>
+      <c r="B54">
+        <v>0.73723702941129698</v>
+      </c>
+      <c r="D54">
+        <v>2.5177318180108901E-2</v>
+      </c>
+      <c r="E54">
+        <v>0.25755480262040298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1.7517140533045001E-2</v>
+      </c>
+      <c r="B55">
+        <v>0.28289037766117697</v>
+      </c>
+      <c r="D55">
+        <v>2.5305717637821499E-2</v>
+      </c>
+      <c r="E55">
+        <v>0.71365139375392295</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1.7629538442124001E-2</v>
+      </c>
+      <c r="B56">
+        <v>0.74086516582693795</v>
+      </c>
+      <c r="D56">
+        <v>2.5412802839651E-2</v>
+      </c>
+      <c r="E56">
+        <v>0.25605076810468402</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1.7788816757524101E-2</v>
+      </c>
+      <c r="B57">
+        <v>0.27474981159677297</v>
+      </c>
+      <c r="D57">
+        <v>2.5586563888509498E-2</v>
+      </c>
+      <c r="E57">
+        <v>0.717674005312675</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1.7904002901500099E-2</v>
+      </c>
+      <c r="B58">
+        <v>0.74478753482951099</v>
+      </c>
+      <c r="D58">
+        <v>2.56948404024782E-2</v>
+      </c>
+      <c r="E58">
+        <v>0.25032695722513398</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1.8066623574625101E-2</v>
+      </c>
+      <c r="B59">
+        <v>0.26876460737070201</v>
+      </c>
+      <c r="D59">
+        <v>2.58673736824588E-2</v>
+      </c>
+      <c r="E59">
+        <v>0.721994878564998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1.8181738520158398E-2</v>
+      </c>
+      <c r="B60">
+        <v>0.74810336831706903</v>
+      </c>
+      <c r="D60">
+        <v>2.59767827073751E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.24538247528685</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1.8353055350490598E-2</v>
+      </c>
+      <c r="B61">
+        <v>0.26196482288908002</v>
+      </c>
+      <c r="D61">
+        <v>2.6185226021988101E-2</v>
+      </c>
+      <c r="E61">
+        <v>0.24017197124575301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1.84722465416195E-2</v>
+      </c>
+      <c r="B62">
+        <v>0.75154752682983195</v>
+      </c>
+      <c r="D62">
+        <v>2.6148211700980001E-2</v>
+      </c>
+      <c r="E62">
+        <v>0.72608483953842695</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1.8635275197011299E-2</v>
+      </c>
+      <c r="B63">
+        <v>0.25474970354167498</v>
+      </c>
+      <c r="D63">
+        <v>2.6438243873799099E-2</v>
+      </c>
+      <c r="E63">
+        <v>0.23646494384407099</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1.8753158649641902E-2</v>
+      </c>
+      <c r="B64">
+        <v>0.75503134307116504</v>
+      </c>
+      <c r="D64">
+        <v>2.64290144387864E-2</v>
+      </c>
+      <c r="E64">
+        <v>0.73046344086047299</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1.8917404489697101E-2</v>
+      </c>
+      <c r="B65">
+        <v>0.24827542775571901</v>
+      </c>
+      <c r="D65">
+        <v>2.6720196762910601E-2</v>
+      </c>
+      <c r="E65">
+        <v>0.23143386980120201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1.9031894651570701E-2</v>
+      </c>
+      <c r="B66">
+        <v>0.758881336382215</v>
+      </c>
+      <c r="D66">
+        <v>2.6709848929236099E-2</v>
+      </c>
+      <c r="E66">
+        <v>0.73458226586876396</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1.9199484389382099E-2</v>
+      </c>
+      <c r="B67">
+        <v>0.24220524845782901</v>
+      </c>
+      <c r="D67">
+        <v>2.70023119433104E-2</v>
+      </c>
+      <c r="E67">
+        <v>0.22507505015469401</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1.9314938372785299E-2</v>
+      </c>
+      <c r="B68">
+        <v>0.76236298310458805</v>
+      </c>
+      <c r="D68">
+        <v>2.6990812782307E-2</v>
+      </c>
+      <c r="E68">
+        <v>0.73764274293212595</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1.9481592513638998E-2</v>
+      </c>
+      <c r="B69">
+        <v>0.23590415688104399</v>
+      </c>
+      <c r="D69">
+        <v>2.7284257776278902E-2</v>
+      </c>
+      <c r="E69">
+        <v>0.22010170418154801</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1.9621487604283699E-2</v>
+      </c>
+      <c r="B70">
+        <v>0.76534817381744902</v>
+      </c>
+      <c r="D70">
+        <v>2.7271627280351599E-2</v>
+      </c>
+      <c r="E70">
+        <v>0.74192513080463296</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1.9763693581752999E-2</v>
+      </c>
+      <c r="B71">
+        <v>0.22966079337398301</v>
+      </c>
+      <c r="D71">
+        <v>2.7566223366447699E-2</v>
+      </c>
+      <c r="E71">
+        <v>0.21496671961317601</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1.9793384949378601E-2</v>
+      </c>
+      <c r="B72">
+        <v>0.77141738289568096</v>
+      </c>
+      <c r="D72">
+        <v>2.75525210424023E-2</v>
+      </c>
+      <c r="E72">
+        <v>0.74555904002724704</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1.9933653198917801E-2</v>
+      </c>
+      <c r="B73">
+        <v>0.76888340271720601</v>
+      </c>
+      <c r="D73">
+        <v>2.78481325074727E-2</v>
+      </c>
+      <c r="E73">
+        <v>0.210293559602591</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.00437347084347E-2</v>
+      </c>
+      <c r="B74">
+        <v>0.224174549485091</v>
+      </c>
+      <c r="D74">
+        <v>2.7833460904587201E-2</v>
+      </c>
+      <c r="E74">
+        <v>0.74881579252766794</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2.0183340044900501E-2</v>
+      </c>
+      <c r="B75">
+        <v>0.77208489402122205</v>
+      </c>
+      <c r="D75">
+        <v>2.8130150313099501E-2</v>
+      </c>
+      <c r="E75">
+        <v>0.20473138731826601</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2.0336437375057401E-2</v>
+      </c>
+      <c r="B76">
+        <v>0.21704099803854399</v>
+      </c>
+      <c r="D76">
+        <v>2.8107913015712999E-2</v>
+      </c>
+      <c r="E76">
+        <v>0.75283918565225605</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2.0464340354710099E-2</v>
+      </c>
+      <c r="B77">
+        <v>0.77484710939101298</v>
+      </c>
+      <c r="D77">
+        <v>2.8412161062583301E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.19922694310366501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2.0610025010666701E-2</v>
+      </c>
+      <c r="B78">
+        <v>0.210699790573906</v>
+      </c>
+      <c r="D78">
+        <v>2.8395199270892499E-2</v>
+      </c>
+      <c r="E78">
+        <v>0.75648578319197002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2.0745277159233001E-2</v>
+      </c>
+      <c r="B79">
+        <v>0.77812887738831404</v>
+      </c>
+      <c r="D79">
+        <v>2.8694092178453499E-2</v>
+      </c>
+      <c r="E79">
+        <v>0.19437400139022801</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2.0902598276975E-2</v>
+      </c>
+      <c r="B80">
+        <v>0.20596621013404301</v>
+      </c>
+      <c r="D80">
+        <v>2.8672075265132602E-2</v>
+      </c>
+      <c r="E80">
+        <v>0.75811587349691201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2.1026242188327798E-2</v>
+      </c>
+      <c r="B81">
+        <v>0.78117973310672195</v>
+      </c>
+      <c r="D81">
+        <v>2.8975954883337599E-2</v>
+      </c>
+      <c r="E81">
+        <v>0.190080747057537</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2.1174128360892799E-2</v>
+      </c>
+      <c r="B82">
+        <v>0.19902125653591099</v>
+      </c>
+      <c r="D82">
+        <v>2.89464059517981E-2</v>
+      </c>
+      <c r="E82">
+        <v>0.76313267048799005</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2.1307193105136599E-2</v>
+      </c>
+      <c r="B83">
+        <v>0.78434604496457605</v>
+      </c>
+      <c r="D83">
+        <v>2.9255764802226799E-2</v>
+      </c>
+      <c r="E83">
+        <v>0.18514475723632601</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2.14560044556482E-2</v>
+      </c>
+      <c r="B84">
+        <v>0.194618456318531</v>
+      </c>
+      <c r="D84">
+        <v>2.9238057901438099E-2</v>
+      </c>
+      <c r="E84">
+        <v>0.76593661204076402</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2.1588129909659401E-2</v>
+      </c>
+      <c r="B85">
+        <v>0.787627812961878</v>
+      </c>
+      <c r="D85">
+        <v>2.95399973155294E-2</v>
+      </c>
+      <c r="E85">
+        <v>0.178900598688155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2.1746675366209799E-2</v>
+      </c>
+      <c r="B86">
+        <v>0.18801143292275799</v>
+      </c>
+      <c r="D86">
+        <v>2.9519037042818799E-2</v>
+      </c>
+      <c r="E86">
+        <v>0.76887201161972496</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2.18799609089275E-2</v>
+      </c>
+      <c r="B87">
+        <v>0.78896690474541997</v>
+      </c>
+      <c r="D87">
+        <v>2.9821974901141302E-2</v>
+      </c>
+      <c r="E87">
+        <v>0.17366747640125299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2.20072252376395E-2</v>
+      </c>
+      <c r="B88">
+        <v>0.18371288819787099</v>
+      </c>
+      <c r="D88">
+        <v>2.97999315104839E-2</v>
+      </c>
+      <c r="E88">
+        <v>0.77250014803536704</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2.2139612172148999E-2</v>
+      </c>
+      <c r="B89">
+        <v>0.79202009842370102</v>
+      </c>
+      <c r="D89">
+        <v>3.00973915478111E-2</v>
+      </c>
+      <c r="E89">
+        <v>0.16979976310615</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2.2291815057782102E-2</v>
+      </c>
+      <c r="B90">
+        <v>0.17803293124691699</v>
+      </c>
+      <c r="D90">
+        <v>3.0080931820293502E-2</v>
+      </c>
+      <c r="E90">
+        <v>0.77526236340515797</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2.24311378952314E-2</v>
+      </c>
+      <c r="B91">
+        <v>0.79585673100152698</v>
+      </c>
+      <c r="D91">
+        <v>3.03858312863633E-2</v>
+      </c>
+      <c r="E91">
+        <v>0.164009424803577</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2.2622943265715598E-2</v>
+      </c>
+      <c r="B92">
+        <v>0.79598722554569101</v>
+      </c>
+      <c r="D92">
+        <v>3.0361946242389099E-2</v>
+      </c>
+      <c r="E92">
+        <v>0.77790912263550105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2.3224641157706699E-2</v>
+      </c>
+      <c r="B93">
+        <v>0.16287071033021</v>
+      </c>
+      <c r="D93">
+        <v>3.06677418386169E-2</v>
+      </c>
+      <c r="E93">
+        <v>0.159324719179049</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2.3430069000218198E-2</v>
+      </c>
+      <c r="B94">
+        <v>0.15617490105540099</v>
+      </c>
+      <c r="D94">
+        <v>3.06428901030549E-2</v>
+      </c>
+      <c r="E94">
+        <v>0.78113316256307896</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2.38917030421451E-2</v>
+      </c>
+      <c r="B95">
+        <v>0.14584303190439901</v>
+      </c>
+      <c r="D95">
+        <v>3.0949655918941901E-2</v>
+      </c>
+      <c r="E95">
+        <v>0.15461114951965799</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2.41736770996855E-2</v>
+      </c>
+      <c r="B96">
+        <v>0.14063877365235899</v>
+      </c>
+      <c r="D96">
+        <v>3.0923848076006701E-2</v>
+      </c>
+      <c r="E96">
+        <v>0.78424174635121102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2.4455637044939901E-2</v>
+      </c>
+      <c r="B97">
+        <v>0.135549971539767</v>
+      </c>
+      <c r="D97">
+        <v>3.1231569999267E-2</v>
+      </c>
+      <c r="E97">
+        <v>0.149897579860267</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2.4737596990194299E-2</v>
+      </c>
+      <c r="B98">
+        <v>0.13046116942717301</v>
+      </c>
+      <c r="D98">
+        <v>3.1204869554245299E-2</v>
+      </c>
+      <c r="E98">
+        <v>0.78683077751183095</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2.5019571047734598E-2</v>
+      </c>
+      <c r="B99">
+        <v>0.12525691117513399</v>
+      </c>
+      <c r="D99">
+        <v>3.1513487607663503E-2</v>
+      </c>
+      <c r="E99">
+        <v>0.14515514616601499</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2.5301552161417998E-2</v>
+      </c>
+      <c r="B100">
+        <v>0.11999492485337</v>
+      </c>
+      <c r="D100">
+        <v>3.1485898088626903E-2</v>
+      </c>
+      <c r="E100">
+        <v>0.78936208060272794</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2.5587617605860698E-2</v>
+      </c>
+      <c r="B101">
+        <v>0.11619218932488801</v>
+      </c>
+      <c r="D101">
+        <v>3.1795313486201397E-2</v>
+      </c>
+      <c r="E101">
+        <v>0.141163177378166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2.5865415602783E-2</v>
+      </c>
+      <c r="B102">
+        <v>0.110279145185972</v>
+      </c>
+      <c r="D102">
+        <v>3.1766877230007602E-2</v>
+      </c>
+      <c r="E102">
+        <v>0.792297480181689</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2.6147368491894401E-2</v>
+      </c>
+      <c r="B103">
+        <v>0.105248071143102</v>
+      </c>
+      <c r="D103">
+        <v>3.2077202870026002E-2</v>
+      </c>
+      <c r="E103">
+        <v>0.13665165596280701</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2.6429342549434701E-2</v>
+      </c>
+      <c r="B104">
+        <v>0.100043812891062</v>
+      </c>
+      <c r="D104">
+        <v>3.2045711205921597E-2</v>
+      </c>
+      <c r="E104">
+        <v>0.79534592382622205</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2.67111665463345E-2</v>
+      </c>
+      <c r="B105">
+        <v>9.6067238255140602E-2</v>
+      </c>
+      <c r="D105">
+        <v>3.23590216924209E-2</v>
+      </c>
+      <c r="E105">
+        <v>0.132717415244682</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2.69932236311572E-2</v>
+      </c>
+      <c r="B106">
+        <v>9.0183713049355199E-2</v>
+      </c>
+      <c r="D106">
+        <v>3.2316380714801897E-2</v>
+      </c>
+      <c r="E106">
+        <v>0.79544154975385595</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2.7285641074308201E-2</v>
+      </c>
+      <c r="B107">
+        <v>8.6724960815885099E-2</v>
+      </c>
+      <c r="D107">
+        <v>3.2640974581532298E-2</v>
+      </c>
+      <c r="E107">
+        <v>0.12768634120181299</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2.7557062376021801E-2</v>
+      </c>
+      <c r="B108">
+        <v>8.0669981625988305E-2</v>
+      </c>
+      <c r="D108">
+        <v>3.2922835740785097E-2</v>
+      </c>
+      <c r="E108">
+        <v>0.123405732065347</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2.78389870405613E-2</v>
+      </c>
+      <c r="B109">
+        <v>7.5869819862012397E-2</v>
+      </c>
+      <c r="D109">
+        <v>3.3204718068466699E-2</v>
+      </c>
+      <c r="E109">
+        <v>0.11895193871971201</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2.8112242998249899E-2</v>
+      </c>
+      <c r="B110">
+        <v>7.2242152385872505E-2</v>
+      </c>
+      <c r="D110">
+        <v>3.3486610980362902E-2</v>
+      </c>
+      <c r="E110">
+        <v>0.114411553269491</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2.8402822257354399E-2</v>
+      </c>
+      <c r="B111">
+        <v>6.6384952473507397E-2</v>
+      </c>
+      <c r="D111">
+        <v>3.3768440386972201E-2</v>
+      </c>
+      <c r="E111">
+        <v>0.110390720446781</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>2.8684753978036898E-2</v>
+      </c>
+      <c r="B112">
+        <v>6.1527062639808103E-2</v>
+      </c>
+      <c r="D112">
+        <v>3.4050343883082798E-2</v>
+      </c>
+      <c r="E112">
+        <v>0.105763742891976</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2.8966664530290499E-2</v>
+      </c>
+      <c r="B113">
+        <v>5.6842357015278899E-2</v>
+      </c>
+      <c r="D113">
+        <v>3.4332254435336398E-2</v>
+      </c>
+      <c r="E113">
+        <v>0.10107903726744601</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2.9248582138687002E-2</v>
+      </c>
+      <c r="B114">
+        <v>5.2099923321026198E-2</v>
+      </c>
+      <c r="D114">
+        <v>3.4614129706875101E-2</v>
+      </c>
+      <c r="E114">
+        <v>9.6682971991534694E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2.9530422129510799E-2</v>
+      </c>
+      <c r="B115">
+        <v>4.7992498393731202E-2</v>
+      </c>
+      <c r="D115">
+        <v>3.4895874943778903E-2</v>
+      </c>
+      <c r="E115">
+        <v>9.3350752571954104E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2.98123115133355E-2</v>
+      </c>
+      <c r="B116">
+        <v>4.3480976978372103E-2</v>
+      </c>
+      <c r="D116">
+        <v>3.5177848497309101E-2</v>
+      </c>
+      <c r="E116">
+        <v>8.8150617753466096E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>3.0094193841017101E-2</v>
+      </c>
+      <c r="B117">
+        <v>3.9027183632736703E-2</v>
+      </c>
+      <c r="D117">
+        <v>3.5459776689920099E-2</v>
+      </c>
+      <c r="E117">
+        <v>8.3321591954628405E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>3.03760832248418E-2</v>
+      </c>
+      <c r="B118">
+        <v>3.4515662217378097E-2</v>
+      </c>
+      <c r="D118">
+        <v>3.5741623736886899E-2</v>
+      </c>
+      <c r="E118">
+        <v>7.9156438957610001E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>3.0657951440237498E-2</v>
+      </c>
+      <c r="B119">
+        <v>3.0177325011189401E-2</v>
+      </c>
+      <c r="D119">
+        <v>3.6023463727710703E-2</v>
+      </c>
+      <c r="E119">
+        <v>7.5049014030314803E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>3.0939756150346401E-2</v>
+      </c>
+      <c r="B120">
+        <v>2.63585404325112E-2</v>
+      </c>
+      <c r="D120">
+        <v>3.6305331943106402E-2</v>
+      </c>
+      <c r="E120">
+        <v>7.0710676824126101E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>3.1221631421885099E-2</v>
+      </c>
+      <c r="B121">
+        <v>2.1962475156599201E-2</v>
+      </c>
+      <c r="D121">
+        <v>3.6587171933930199E-2</v>
+      </c>
+      <c r="E121">
+        <v>6.6603251896830903E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>3.1503485524994899E-2</v>
+      </c>
+      <c r="B122">
+        <v>1.7739594089857001E-2</v>
+      </c>
+      <c r="D122">
+        <v>3.68690683738978E-2</v>
+      </c>
+      <c r="E122">
+        <v>6.2034002411748702E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>3.17853325719617E-2</v>
+      </c>
+      <c r="B123">
+        <v>1.3574441092838599E-2</v>
+      </c>
+      <c r="D123">
+        <v>3.7150908364721603E-2</v>
+      </c>
+      <c r="E123">
+        <v>5.7926577484453699E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>3.20675274867772E-2</v>
+      </c>
+      <c r="B124">
+        <v>6.5632942584563604E-3</v>
+      </c>
+      <c r="D124">
+        <v>3.7432736595307103E-2</v>
+      </c>
+      <c r="E124">
+        <v>5.3915366006697697E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>3.2349303737109397E-2</v>
+      </c>
+      <c r="B125">
+        <v>2.9773462276629901E-3</v>
+      </c>
+      <c r="D125">
+        <v>3.7714581290226298E-2</v>
+      </c>
+      <c r="E125">
+        <v>4.9769455699587101E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>3.2618115147939698E-2</v>
+      </c>
+      <c r="B126">
+        <v>8.3744591762124898E-4</v>
+      </c>
+      <c r="D126">
+        <v>3.7996414224907099E-2</v>
+      </c>
+      <c r="E126">
+        <v>4.5719758842015498E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>3.8278240103445001E-2</v>
+      </c>
+      <c r="E127">
+        <v>4.1727790054167199E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>3.85600942065547E-2</v>
+      </c>
+      <c r="E128">
+        <v>3.7504908987425499E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>3.8841934197378497E-2</v>
+      </c>
+      <c r="E129">
+        <v>3.3397484060130302E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>3.9123753019773402E-2</v>
+      </c>
+      <c r="E130">
+        <v>2.94632433420054E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>3.9405593010597199E-2</v>
+      </c>
+      <c r="E131">
+        <v>2.53558184147104E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>3.9687433001421003E-2</v>
+      </c>
+      <c r="E132">
+        <v>2.1248393487415401E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>3.9969251823815902E-2</v>
+      </c>
+      <c r="E133">
+        <v>1.7314152769290599E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>4.0251105926925698E-2</v>
+      </c>
+      <c r="E134">
+        <v>1.3091271702548601E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>4.0532903580891601E-2</v>
+      </c>
+      <c r="E135">
+        <v>9.3302151935941106E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>4.0814792964716302E-2</v>
+      </c>
+      <c r="E136">
+        <v>4.8186937782355097E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>4.0994356515148801E-2</v>
+      </c>
+      <c r="E137">
+        <v>4.8003316549372001E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C880236A-8313-45CB-937D-1F7FCDCED26D}">
   <dimension ref="A1:C158"/>
   <sheetViews>
@@ -34364,7 +36905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AD2FA9-8674-4C65-A2F1-A6D0908A8068}">
   <dimension ref="A1:Z98"/>
   <sheetViews>
@@ -39278,667 +41819,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596094CB-5E7C-4458-92EE-C2DA16EDDB8D}">
-  <dimension ref="A1:B81"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4.0465455966455597</v>
-      </c>
-      <c r="B2">
-        <v>1.3971791027042799</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4.0543895497041298</v>
-      </c>
-      <c r="B3">
-        <v>1.3907254301576699</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4.0959568161710198</v>
-      </c>
-      <c r="B4">
-        <v>1.38546817295806</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4.1513567102403002</v>
-      </c>
-      <c r="B5">
-        <v>1.37970492324917</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4.1887808578635397</v>
-      </c>
-      <c r="B6">
-        <v>1.37440870669709</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4.2253637958448804</v>
-      </c>
-      <c r="B7">
-        <v>1.3695735934192801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4.2620241853533498</v>
-      </c>
-      <c r="B8">
-        <v>1.36488312691928</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4.2987878435646696</v>
-      </c>
-      <c r="B9">
-        <v>1.3603855227897099</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4.3355773189516897</v>
-      </c>
-      <c r="B10">
-        <v>1.3559361342527501</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4.3722358643761901</v>
-      </c>
-      <c r="B11">
-        <v>1.35124222378185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4.3967685433905999</v>
-      </c>
-      <c r="B12">
-        <v>1.3476782080568099</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4.44748177486332</v>
-      </c>
-      <c r="B13">
-        <v>1.3436277090033399</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4.4872360147985999</v>
-      </c>
-      <c r="B14">
-        <v>1.33841565308246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4.51990826535451</v>
-      </c>
-      <c r="B15">
-        <v>1.3344055375152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4.5578610503851396</v>
-      </c>
-      <c r="B16">
-        <v>1.33009659262123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4.6066711592505696</v>
-      </c>
-      <c r="B17">
-        <v>1.3251890514898901</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4.65440201237897</v>
-      </c>
-      <c r="B18">
-        <v>1.3203904134073601</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4.70081742172954</v>
-      </c>
-      <c r="B19">
-        <v>1.3156290565734099</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4.7474290416155096</v>
-      </c>
-      <c r="B20">
-        <v>1.31123413824325</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4.7939787002797702</v>
-      </c>
-      <c r="B21">
-        <v>1.3067235024908499</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>4.8408484919228396</v>
-      </c>
-      <c r="B22">
-        <v>1.3028107400867499</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>4.9003374178526702</v>
-      </c>
-      <c r="B23">
-        <v>1.29747002243305</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>4.9629700998502004</v>
-      </c>
-      <c r="B24">
-        <v>1.2938268365648</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>5.0157660634112498</v>
-      </c>
-      <c r="B25">
-        <v>1.2883199425843199</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>5.0783802662936699</v>
-      </c>
-      <c r="B26">
-        <v>1.2819716837888899</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>5.1661822485718503</v>
-      </c>
-      <c r="B27">
-        <v>1.27680846732852</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>5.2223169844946096</v>
-      </c>
-      <c r="B28">
-        <v>1.2724901681905101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>5.2862296847862797</v>
-      </c>
-      <c r="B29">
-        <v>1.26752284334673</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>5.3654502752069897</v>
-      </c>
-      <c r="B30">
-        <v>1.26227214688423</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>5.4471003205374497</v>
-      </c>
-      <c r="B31">
-        <v>1.2572120046486399</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>5.5240129141250698</v>
-      </c>
-      <c r="B32">
-        <v>1.2527101507699101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>5.5626644533101999</v>
-      </c>
-      <c r="B33">
-        <v>1.24781920784962</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>5.66157500174796</v>
-      </c>
-      <c r="B34">
-        <v>1.2452567175346401</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>5.7136494577803303</v>
-      </c>
-      <c r="B35">
-        <v>1.24108817140108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>5.80422931213654</v>
-      </c>
-      <c r="B36">
-        <v>1.2365061819624199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>5.8851306593714003</v>
-      </c>
-      <c r="B37">
-        <v>1.2321379763412601</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>5.9709103770998198</v>
-      </c>
-      <c r="B38">
-        <v>1.2277359327395401</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>6.0548488999138499</v>
-      </c>
-      <c r="B39">
-        <v>1.2235531441918299</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>6.1026027454165899</v>
-      </c>
-      <c r="B40">
-        <v>1.22024632703739</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>6.1903470477674496</v>
-      </c>
-      <c r="B41">
-        <v>1.2169005627012399</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>6.2811164367025096</v>
-      </c>
-      <c r="B42">
-        <v>1.21267254389598</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>6.3768077984723401</v>
-      </c>
-      <c r="B43">
-        <v>1.20849211788877</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>6.4724681796313197</v>
-      </c>
-      <c r="B44">
-        <v>1.20425383317044</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>6.56813888766058</v>
-      </c>
-      <c r="B45">
-        <v>1.2000348346891501</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>6.67859241270917</v>
-      </c>
-      <c r="B46">
-        <v>1.19599017389903</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>6.75531848279042</v>
-      </c>
-      <c r="B47">
-        <v>1.192968888</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>6.8605939178174697</v>
-      </c>
-      <c r="B48">
-        <v>1.18839831555637</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>6.9661374658907</v>
-      </c>
-      <c r="B49">
-        <v>1.1843284651728301</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>7.0683889178465797</v>
-      </c>
-      <c r="B50">
-        <v>1.1811446573258899</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>7.1964876956409398</v>
-      </c>
-      <c r="B51">
-        <v>1.1755858673430899</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>7.30212512435312</v>
-      </c>
-      <c r="B52">
-        <v>1.1716913463872101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>7.4077813291930896</v>
-      </c>
-      <c r="B53">
-        <v>1.1678318913168599</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>7.5134656982247501</v>
-      </c>
-      <c r="B54">
-        <v>1.1640250350748</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>7.6192627240231303</v>
-      </c>
-      <c r="B55">
-        <v>1.1604285741459399</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>7.7250221975659503</v>
-      </c>
-      <c r="B56">
-        <v>1.1567619814460099</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>7.8308192233643403</v>
-      </c>
-      <c r="B57">
-        <v>1.1531655205171401</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>7.9331539007741103</v>
-      </c>
-      <c r="B58">
-        <v>1.14919923747657</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>8.0555112940146003</v>
-      </c>
-      <c r="B59">
-        <v>1.14561318052453</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>8.1469655154753902</v>
-      </c>
-      <c r="B60">
-        <v>1.1432789013753599</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>8.2543546849219993</v>
-      </c>
-      <c r="B61">
-        <v>1.1394283956840101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>8.3602737555510203</v>
-      </c>
-      <c r="B62">
-        <v>1.1360598630111001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>8.4663148710106704</v>
-      </c>
-      <c r="B63">
-        <v>1.1329192585941401</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>8.5723090461508509</v>
-      </c>
-      <c r="B64">
-        <v>1.12969098946335</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>8.6783877138660799</v>
-      </c>
-      <c r="B65">
-        <v>1.1266205168174599</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>8.7844476054535097</v>
-      </c>
-      <c r="B66">
-        <v>1.1235149782860301</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>8.8904981089770594</v>
-      </c>
-      <c r="B67">
-        <v>1.12039190681184</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>9.0007393562100599</v>
-      </c>
-      <c r="B68">
-        <v>1.1174748966169099</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>9.1016620698966708</v>
-      </c>
-      <c r="B69">
-        <v>1.11405840719547</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>9.2088937092089491</v>
-      </c>
-      <c r="B70">
-        <v>1.11147854890117</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>9.3150287053075491</v>
-      </c>
-      <c r="B71">
-        <v>1.1085132739118699</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>9.4211918655978302</v>
-      </c>
-      <c r="B72">
-        <v>1.1056005977508601</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>9.5198648503826302</v>
-      </c>
-      <c r="B73">
-        <v>1.1029243296634199</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>9.6181313099348404</v>
-      </c>
-      <c r="B74">
-        <v>1.0991762088674</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>9.7301530483696297</v>
-      </c>
-      <c r="B75">
-        <v>1.0973568801696001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>9.8427682590989996</v>
-      </c>
-      <c r="B76">
-        <v>1.0949428689016301</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>9.9425263092696596</v>
-      </c>
-      <c r="B77">
-        <v>1.09161919256142</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>10.046718772450999</v>
-      </c>
-      <c r="B78">
-        <v>1.08894518958888</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>10.1839726437893</v>
-      </c>
-      <c r="B79">
-        <v>1.0853102852718099</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>10.290257848910199</v>
-      </c>
-      <c r="B80">
-        <v>1.0826255373667499</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>10.358126314235699</v>
-      </c>
-      <c r="B81">
-        <v>1.0813511345859499</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed 4 engine plot, found correct code value
</commit_message>
<xml_diff>
--- a/MAE 159/Other data/159 Digitized Plots.xlsx
+++ b/MAE 159/Other data/159 Digitized Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy Slagle\Documents\MAE136-MAE158-MAE159_Aircraft_Design_and_Analysis_Course_Series\MAE 159\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60630B69-B0AD-4CD6-B05B-F003EB9EC074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D61738-F0CA-4D33-8F97-A524D598C978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="2430" windowWidth="28800" windowHeight="15435" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="4050" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 1a" sheetId="6" r:id="rId1"/>
@@ -10106,7 +10106,7 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -10115,6 +10115,698 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2, TOFL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Figure 5'!$B$2:$B$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="146"/>
+                <c:pt idx="0">
+                  <c:v>70.643408757290402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.849330145099202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.730029234863494</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.9231356523551</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.0590994881303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.805084108819997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.866074447708598</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.069275991755006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>87.273732029126506</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89.495013201355704</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.680910389834395</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>93.885639050543006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96.889420627219707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>103.518211887381</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>105.79077461991101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>107.90742403547399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>110.078667795646</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>112.31453850008801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>114.517648459732</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>116.72056673109201</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>118.924635132156</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>122.930144385839</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>124.731457446269</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>126.93642039265799</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>129.13981788472799</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>132.75878834573899</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>134.94897240629601</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>136.949152020523</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>139.15427257727899</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>140.89974349365201</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>142.958425459343</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>145.16077931520101</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>147.36454953448899</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>153.05531257967499</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>157.578134884695</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>160.29662024660601</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>162.780124099647</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>164.82672967302199</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>167.47878556154799</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>170.278978213877</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>173.28197341218799</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>176.00057017933099</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>182.60887772074901</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>185.0147987531</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>187.08163160382099</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>189.32745026120301</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>191.41918555963301</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>195.62314604249801</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>197.825723534687</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>200.028782377455</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>203.23167544295899</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>207.808437298884</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>209.91383032527199</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>211.32340145521701</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>213.242669097049</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>215.38980455644</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>216.84025126019699</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>225.05132308482499</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>227.16719814057399</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>229.275148910328</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>230.176268792553</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>232.064260784787</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>234.26688034190499</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>236.46822250959701</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>238.61930106798499</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>240.70217431968999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>242.997841776396</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>245.278255595274</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>246.67737240589901</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>248.682421967473</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>250.972523417318</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>253.18632228079699</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>255.489274452345</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>257.11067101931701</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>258.22512114384199</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>259.46591902560198</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>261.21069050793898</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>263.49709815497903</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>265.73327267013701</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>267.90127339923799</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>270.105014459595</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>272.46720819956897</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>274.47607124234798</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>276.67915990329402</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>278.84698438566699</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>281.04879326108397</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>283.11513739542499</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>284.18605172568999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>286.31984830482202</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>288.43494356741598</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>290.85664491394402</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>293.20860873702998</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>295.32602490572901</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>297.57982449935298</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>299.81948698785601</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>301.93237296691098</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>304.13314858923002</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>306.33484005557301</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>308.53727271661398</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>310.675024578104</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>312.19969554125498</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>314.34300879711799</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>316.54432966611103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>318.74648118433601</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>320.05628270811701</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>321.74884000797101</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>323.90307472136601</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>325.35170041451198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Figure 5'!$C$2:$C$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="146"/>
+                <c:pt idx="0">
+                  <c:v>2983.6960333294801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3037.7469948995199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3115.0315235173102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3164.8029015226598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3239.4017004268599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3312.0036189612597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3355.9567345892096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3429.4011535583404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3493.9005870865399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3557.9994234788101</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3635.2614543957702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3697.81698616431</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3802.1337731171602</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4005.2281432322002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4062.3770099664098</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4155.1258996127999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4217.3034843514597</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4296.94236889695</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4371.0398173634703</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4446.5040717547399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4513.76749059745</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4649.5255832068397</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4718.9314609233497</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4779.8164521171902</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4851.8636916965606</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4984.5055015541602</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5040.3981899378896</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5126.6379958318503</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5186.3991688208798</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5262.6639825980901</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5323.0766235421997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5402.5653620452595</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5471.9549234376</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5667.6825673222102</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5821.4411739097095</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5927.3552662437696</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6034.8107115181701</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6076.9815440922202</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6170.3157714090503</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6268.6958428940397</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6378.61978843822</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6466.6582897717399</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6696.2402667699998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6759.0458148289099</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6848.2987332972698</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6912.1906790208695</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7007.8319798658804</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7163.3854134896901</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7241.2795450805406</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7315.7414751269898</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7435.1457160201007</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7597.1643944813995</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7676.2285835743005</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7746.1129160451201</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7794.3596334525801</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7876.2597649278296</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7969.1366087857796</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8249.0246748344907</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8292.9456522481705</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8373.3021576444207</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8437.8125422811499</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8463.0960716781792</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8540.6902653021989</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8627.3927017415008</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>8713.7867536772901</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8774.0720439686902</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8866.1949949100908</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8940.9435033295304</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9008.5053226392902</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9060.0206646781098</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9151.5370442986896</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9229.1312065451693</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9308.7297664609196</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9405.5339529697503</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9410.4200017528401</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9470.9504042588997</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9525.0277453805193</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>9603.0260504256803</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9680.4986560570887</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9765.8002105561409</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9835.3976855481505</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9923.0297490395806</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9995.1810574814499</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>10069.430373272899</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>10155.9886298861</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10239.3632735669</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10332.1009143629</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10408.275477962699</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>10438.543279069499</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>10525.2926025283</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10612.2287299688</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10701.0625803855</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10788.344246332899</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10859.712371214498</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>10929.395713103799</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>11031.898017228701</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11122.6401245122</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>11206.851936822</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>11285.7787662226</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>11347.628303195301</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11428.665711882599</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11498.687970122201</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>11585.5422738865</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>11666.4737519768</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>11755.961116001601</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11780.9352762378</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11872.417575015599</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>11918.076491096101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4358-422D-8D72-905B9DE39A84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Figure 5'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4, TOFL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10141,713 +10833,854 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Figure 5'!$B$2:$B$147</c:f>
+              <c:f>'Figure 5'!$I$2:$I$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="146"/>
                 <c:pt idx="0">
-                  <c:v>70.643408757290402</c:v>
+                  <c:v>70.634700480256797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.849330145099202</c:v>
+                  <c:v>72.941308573354306</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.730029234863494</c:v>
+                  <c:v>74.824118364111897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.9231356523551</c:v>
+                  <c:v>76.950332112243402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.0590994881303</c:v>
+                  <c:v>78.971155362940394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.805084108819997</c:v>
+                  <c:v>81.026507378587695</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>82.866074447708598</c:v>
+                  <c:v>83.199702581272106</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>85.069275991755006</c:v>
+                  <c:v>85.416611109023805</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.273732029126506</c:v>
+                  <c:v>87.355972388289103</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89.495013201355704</c:v>
+                  <c:v>101.990844965436</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>91.680910389834395</c:v>
+                  <c:v>104.161748631037</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>93.885639050543006</c:v>
+                  <c:v>106.36565310819201</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96.889420627219707</c:v>
+                  <c:v>111.04686508418099</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>103.518211887381</c:v>
+                  <c:v>113.12954596662399</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.79077461991101</c:v>
+                  <c:v>117.03954516362001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>107.90742403547399</c:v>
+                  <c:v>119.244252525631</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>110.078667795646</c:v>
+                  <c:v>120.75571444183601</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>112.31453850008801</c:v>
+                  <c:v>122.917277081577</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>114.517648459732</c:v>
+                  <c:v>125.056569903884</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>116.72056673109201</c:v>
+                  <c:v>127.25787259798901</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>118.924635132156</c:v>
+                  <c:v>129.497934551546</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>122.930144385839</c:v>
+                  <c:v>131.669648353703</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>124.731457446269</c:v>
+                  <c:v>133.87445688452999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>126.93642039265799</c:v>
+                  <c:v>136.045696080694</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>129.13981788472799</c:v>
+                  <c:v>138.28487797204099</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>132.75878834573899</c:v>
+                  <c:v>140.38209844983101</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>134.94897240629601</c:v>
+                  <c:v>142.77746614105101</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>136.949152020523</c:v>
+                  <c:v>144.86542291388801</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>139.15427257727899</c:v>
+                  <c:v>146.96897056201999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>140.89974349365201</c:v>
+                  <c:v>149.108985942663</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>142.958425459343</c:v>
+                  <c:v>151.12798025639501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>145.16077931520101</c:v>
+                  <c:v>153.11744719591999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>147.36454953448899</c:v>
+                  <c:v>155.064278439384</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>153.05531257967499</c:v>
+                  <c:v>157.125286527188</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>157.578134884695</c:v>
+                  <c:v>159.21696078495299</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>160.29662024660601</c:v>
+                  <c:v>159.72994845101701</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>162.780124099647</c:v>
+                  <c:v>161.60109056133399</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>164.82672967302199</c:v>
+                  <c:v>164.481464061152</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>167.47878556154799</c:v>
+                  <c:v>168.79050068280799</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>170.278978213877</c:v>
+                  <c:v>171.00945562425801</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>173.28197341218799</c:v>
+                  <c:v>173.15655652759801</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>176.00057017933099</c:v>
+                  <c:v>175.17684961819899</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>182.60887772074901</c:v>
+                  <c:v>177.27449161517001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>185.0147987531</c:v>
+                  <c:v>179.31781161025299</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>187.08163160382099</c:v>
+                  <c:v>181.57408959583401</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>189.32745026120301</c:v>
+                  <c:v>183.77817561903501</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>191.41918555963301</c:v>
+                  <c:v>186.03263128863</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>195.62314604249801</c:v>
+                  <c:v>185.33227760514001</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>197.825723534687</c:v>
+                  <c:v>188.18696570801899</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>200.028782377455</c:v>
+                  <c:v>189.134683993951</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>203.23167544295899</c:v>
+                  <c:v>190.98955719505699</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>207.808437298884</c:v>
+                  <c:v>193.19508178343699</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>209.91383032527199</c:v>
+                  <c:v>195.20092388186001</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>211.32340145521701</c:v>
+                  <c:v>197.63624334254999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>213.242669097049</c:v>
+                  <c:v>199.17950578090401</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>215.38980455644</c:v>
+                  <c:v>200.946144951208</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>216.84025126019699</c:v>
+                  <c:v>203.214733849862</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>225.05132308482499</c:v>
+                  <c:v>204.97555248646401</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>227.16719814057399</c:v>
+                  <c:v>207.07669857090099</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>229.275148910328</c:v>
+                  <c:v>209.22606474292999</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>230.176268792553</c:v>
+                  <c:v>213.23213628224599</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>232.064260784787</c:v>
+                  <c:v>214.981487466456</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>234.26688034190499</c:v>
+                  <c:v>217.03912402104299</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>236.46822250959701</c:v>
+                  <c:v>219.242920863705</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>238.61930106798499</c:v>
+                  <c:v>221.447005238792</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>240.70217431968999</c:v>
+                  <c:v>223.650945847667</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>242.997841776396</c:v>
+                  <c:v>226.25514984948401</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>245.278255595274</c:v>
+                  <c:v>228.19275936515399</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>246.67737240589901</c:v>
+                  <c:v>230.30274289670899</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>248.682421967473</c:v>
+                  <c:v>231.86640903789399</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>250.972523417318</c:v>
+                  <c:v>235.003858277983</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>253.18632228079699</c:v>
+                  <c:v>237.18698424502301</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>255.489274452345</c:v>
+                  <c:v>238.73818654738801</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>257.11067101931701</c:v>
+                  <c:v>241.09370948437001</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>258.22512114384199</c:v>
+                  <c:v>245.030382866747</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>259.46591902560198</c:v>
+                  <c:v>247.091912772657</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>261.21069050793898</c:v>
+                  <c:v>248.97351364930401</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>263.49709815497903</c:v>
+                  <c:v>251.01406896232999</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>265.73327267013701</c:v>
+                  <c:v>253.301873803972</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>267.90127339923799</c:v>
+                  <c:v>255.52158153487099</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>270.105014459595</c:v>
+                  <c:v>257.70894567118899</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>272.46720819956897</c:v>
+                  <c:v>259.824782304763</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>274.47607124234798</c:v>
+                  <c:v>259.912864981366</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>276.67915990329402</c:v>
+                  <c:v>262.11593411850498</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>278.84698438566699</c:v>
+                  <c:v>264.32075684846399</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>281.04879326108397</c:v>
+                  <c:v>266.52392005485399</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>283.11513739542499</c:v>
+                  <c:v>268.66104626708398</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>284.18605172568999</c:v>
+                  <c:v>270.86487627486099</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>286.31984830482202</c:v>
+                  <c:v>272.61371261375302</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>288.43494356741598</c:v>
+                  <c:v>274.75482378706499</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>290.85664491394402</c:v>
+                  <c:v>277.37537885021499</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>293.20860873702998</c:v>
+                  <c:v>279.36329898445899</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>295.32602490572901</c:v>
+                  <c:v>281.349085851231</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>297.57982449935298</c:v>
+                  <c:v>283.55319684969197</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>299.81948698785601</c:v>
+                  <c:v>285.79187715669599</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>301.93237296691098</c:v>
+                  <c:v>287.96236663868302</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>304.13314858923002</c:v>
+                  <c:v>290.074103661636</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>306.33484005557301</c:v>
+                  <c:v>292.165479433359</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>308.53727271661398</c:v>
+                  <c:v>294.37153287309701</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>310.675024578104</c:v>
+                  <c:v>296.56262966479102</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>312.19969554125498</c:v>
+                  <c:v>298.77822136374499</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>314.34300879711799</c:v>
+                  <c:v>300.84502999987501</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>316.54432966611103</c:v>
+                  <c:v>303.18536138679701</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>318.74648118433601</c:v>
+                  <c:v>305.45632778189503</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>320.05628270811701</c:v>
+                  <c:v>307.59177938397801</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>321.74884000797101</c:v>
+                  <c:v>309.830951843045</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>323.90307472136601</c:v>
+                  <c:v>311.42250885774598</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>325.35170041451198</c:v>
+                  <c:v>313.40157286649298</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>315.40345424670699</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>317.60817225806699</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>319.81167411375799</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>322.031523126021</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>324.218396682324</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>326.53206900359902</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>328.625702835222</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>330.720135368027</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>333.03243392326698</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>335.03495071464499</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>341.70761886518301</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>343.69744619643001</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>345.77332245295997</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>348.05489868925298</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>350.25900436303903</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>352.46085663455301</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>354.63316822017299</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>357.01011165974103</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>359.15716195359499</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>361.27525321496103</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>363.47896866616901</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>365.75033334692398</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>367.88589144249801</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>370.12306220426598</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>372.29396434853101</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>374.49655249006901</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>376.69992868344099</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>378.90342201965302</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>381.02547187228299</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>383.708733903481</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>385.41536968632499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Figure 5'!$C$2:$C$147</c:f>
+              <c:f>'Figure 5'!$J$2:$J$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="146"/>
                 <c:pt idx="0">
-                  <c:v>2983.6960333294801</c:v>
+                  <c:v>2328.3774184182803</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3037.7469948995199</c:v>
+                  <c:v>2381.9079520023697</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3115.0315235173102</c:v>
+                  <c:v>2444.14242871531</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3164.8029015226598</c:v>
+                  <c:v>2492.60793599116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3239.4017004268599</c:v>
+                  <c:v>2551.2198645035601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3312.0036189612597</c:v>
+                  <c:v>2602.7666139722496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3355.9567345892096</c:v>
+                  <c:v>2651.0297166491</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3429.4011535583404</c:v>
+                  <c:v>2695.0633740922003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3493.9005870865399</c:v>
+                  <c:v>2748.0726235315597</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3557.9994234788101</c:v>
+                  <c:v>3178.1746939763698</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3635.2614543957702</c:v>
+                  <c:v>3242.7772744648701</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3697.81698616431</c:v>
+                  <c:v>3311.2095293265802</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3802.1337731171602</c:v>
+                  <c:v>3471.4951362455404</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4005.2281432322002</c:v>
+                  <c:v>3507.5302402172401</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4062.3770099664098</c:v>
+                  <c:v>3606.8974074778198</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4155.1258996127999</c:v>
+                  <c:v>3669.6048065713399</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4217.3034843514597</c:v>
+                  <c:v>3733.23005567788</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4296.94236889695</c:v>
+                  <c:v>3784.72507104325</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4371.0398173634703</c:v>
+                  <c:v>3835.58700705413</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4446.5040717547399</c:v>
+                  <c:v>3922.5709042690401</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4513.76749059745</c:v>
+                  <c:v>3972.32468574632</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4649.5255832068397</c:v>
+                  <c:v>4031.15070325837</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4718.9314609233497</c:v>
+                  <c:v>4093.1367325582596</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4779.8164521171902</c:v>
+                  <c:v>4155.3468602951298</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4851.8636916965606</c:v>
+                  <c:v>4211.3757996403101</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4984.5055015541602</c:v>
+                  <c:v>4267.9058126571199</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5040.3981899378896</c:v>
+                  <c:v>4341.5773471350003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5126.6379958318503</c:v>
+                  <c:v>4399.7777800436597</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5186.3991688208798</c:v>
+                  <c:v>4466.3783272985702</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5262.6639825980901</c:v>
+                  <c:v>4512.08816430973</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5323.0766235421997</c:v>
+                  <c:v>4583.7410665736907</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5402.5653620452595</c:v>
+                  <c:v>4626.7974456778202</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5471.9549234376</c:v>
+                  <c:v>4702.1146934113203</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5667.6825673222102</c:v>
+                  <c:v>4745.9412529351303</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5821.4411739097095</c:v>
+                  <c:v>4831.9840648872705</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5927.3552662437696</c:v>
+                  <c:v>4826.4767463888402</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6034.8107115181701</c:v>
+                  <c:v>4876.25105296519</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6076.9815440922202</c:v>
+                  <c:v>4972.2874428649602</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6170.3157714090503</c:v>
+                  <c:v>5096.02221997574</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6268.6958428940397</c:v>
+                  <c:v>5159.6266807106404</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6378.61978843822</c:v>
+                  <c:v>5223.1391379967499</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6466.6582897717399</c:v>
+                  <c:v>5285.5312973399496</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6696.2402667699998</c:v>
+                  <c:v>5329.8581416351299</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6759.0458148289099</c:v>
+                  <c:v>5412.0119763995999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6848.2987332972698</c:v>
+                  <c:v>5465.7082814839505</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6912.1906790208695</c:v>
+                  <c:v>5532.8460481946904</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7007.8319798658804</c:v>
+                  <c:v>5632.1457416411495</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7163.3854134896901</c:v>
+                  <c:v>5571.4258248668502</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7241.2795450805406</c:v>
+                  <c:v>5662.7147172754303</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7315.7414751269898</c:v>
+                  <c:v>5720.5564002359697</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7435.1457160201007</c:v>
+                  <c:v>5766.7652164388101</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7597.1643944813995</c:v>
+                  <c:v>5823.6454996505399</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7676.2285835743005</c:v>
+                  <c:v>5869.5097709113397</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7746.1129160451201</c:v>
+                  <c:v>5961.8312722266901</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7794.3596334525801</c:v>
+                  <c:v>6017.9165839489106</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7876.2597649278296</c:v>
+                  <c:v>6072.4284690050799</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7969.1366087857796</c:v>
+                  <c:v>6121.1218448507998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>8249.0246748344907</c:v>
+                  <c:v>6192.3027306487693</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>8292.9456522481705</c:v>
+                  <c:v>6255.5298064601302</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>8373.3021576444207</c:v>
+                  <c:v>6302.8900889687302</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>8437.8125422811499</c:v>
+                  <c:v>6434.6388841988191</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>8463.0960716781792</c:v>
+                  <c:v>6515.8456270452298</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8540.6902653021989</c:v>
+                  <c:v>6551.1027979661794</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>8627.3927017415008</c:v>
+                  <c:v>6620.3025252023099</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>8713.7867536772901</c:v>
+                  <c:v>6687.4520435512904</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>8774.0720439686902</c:v>
+                  <c:v>6755.62666634385</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>8866.1949949100908</c:v>
+                  <c:v>6839.4273072844799</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>8940.9435033295304</c:v>
+                  <c:v>6893.5397688456305</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>9008.5053226392902</c:v>
+                  <c:v>6962.0776181162601</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>9060.0206646781098</c:v>
+                  <c:v>7004.2027273295698</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>9151.5370442986896</c:v>
+                  <c:v>7111.9703227118798</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>9229.1312065451693</c:v>
+                  <c:v>7191.9109202968202</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>9308.7297664609196</c:v>
+                  <c:v>7268.2477095473205</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9405.5339529697503</c:v>
+                  <c:v>7342.5736816356903</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>9410.4200017528401</c:v>
+                  <c:v>7447.4021279765093</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>9470.9504042588997</c:v>
+                  <c:v>7487.5079380384695</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>9525.0277453805193</c:v>
+                  <c:v>7558.3624041168896</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>9603.0260504256803</c:v>
+                  <c:v>7619.7600291141398</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>9680.4986560570887</c:v>
+                  <c:v>7687.7958376410506</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>9765.8002105561409</c:v>
+                  <c:v>7763.11387266572</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>9835.3976855481505</c:v>
+                  <c:v>7829.9160415751503</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>9923.0297490395806</c:v>
+                  <c:v>7928.4603570839899</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>9995.1810574814499</c:v>
+                  <c:v>7898.2425316926701</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>10069.430373272899</c:v>
+                  <c:v>7972.6310591987203</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>10155.9886298861</c:v>
+                  <c:v>8034.5158436152997</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>10239.3632735669</c:v>
+                  <c:v>8108.2336237693798</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>10332.1009143629</c:v>
+                  <c:v>8174.5442634131605</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>10408.275477962699</c:v>
+                  <c:v>8243.5075115289692</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>10438.543279069499</c:v>
+                  <c:v>8304.4715606924201</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>10525.2926025283</c:v>
+                  <c:v>8366.2817293034695</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>10612.2287299688</c:v>
+                  <c:v>8453.0620866498593</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>10701.0625803855</c:v>
+                  <c:v>8507.1477398329589</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>10788.344246332899</c:v>
+                  <c:v>8576.4443519676097</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>10859.712371214498</c:v>
+                  <c:v>8643.4040361603693</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>10929.395713103799</c:v>
+                  <c:v>8703.009451008671</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>11031.898017228701</c:v>
+                  <c:v>8770.5653085845988</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>11122.6401245122</c:v>
+                  <c:v>8843.9919377073711</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>11206.851936822</c:v>
+                  <c:v>8932.1630617423507</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>11285.7787662226</c:v>
+                  <c:v>8985.2724458975608</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>11347.628303195301</c:v>
+                  <c:v>9034.6570353010811</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>11428.665711882599</c:v>
+                  <c:v>9130.1262616811691</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>11498.687970122201</c:v>
+                  <c:v>9182.7614931801309</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>11585.5422738865</c:v>
+                  <c:v>9271.7604901753493</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>11666.4737519768</c:v>
+                  <c:v>9340.291812916319</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>11755.961116001601</c:v>
+                  <c:v>9418.5430209861297</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>11780.9352762378</c:v>
+                  <c:v>9474.6392158609397</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>11872.417575015599</c:v>
+                  <c:v>9545.0728202873997</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>11918.076491096101</c:v>
+                  <c:v>9602.5214994782509</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>9676.6271061068492</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>9739.2585715378791</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>9810.5616612248796</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>9884.8723096605609</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>9955.1724892885395</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>10013.518071509001</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>10095.6221526479</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>10172.0312091003</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>10240.172233781599</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>10309.747131881799</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>10558.689473426799</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>10599.1761308362</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>10669.934268168801</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>10736.394325275302</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>10803.391976299301</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>10886.4571903055</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>10941.0207982299</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>11008.100030874801</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>11086.426701943899</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>11168.8947160729</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>11238.674793443699</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>11304.366197207701</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>11381.8580686526</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>11452.2270801584</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>11516.840508313</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>11594.6587062414</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>11666.8578131457</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>11738.2216497627</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>11816.3772190708</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>11910.3952677173</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>11937.4722076786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10855,7 +11688,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5903-4139-80BB-FA9FC4942AFC}"/>
+              <c16:uniqueId val="{00000006-4358-422D-8D72-905B9DE39A84}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10867,11 +11700,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="473799624"/>
-        <c:axId val="473799952"/>
+        <c:axId val="597124544"/>
+        <c:axId val="597121592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="473799624"/>
+        <c:axId val="597124544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10928,12 +11761,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473799952"/>
+        <c:crossAx val="597121592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="473799952"/>
+        <c:axId val="597121592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10990,44 +11823,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473799624"/>
+        <c:crossAx val="597124544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -13900,46 +14705,6 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -17075,522 +17840,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -30007,10 +30256,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB30471-B599-4A7E-AA66-1ED16431E92A}">
-  <dimension ref="B1:J147"/>
+  <dimension ref="B1:J140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33070,62 +33319,6 @@
         <v>11937.4722076786</v>
       </c>
     </row>
-    <row r="141" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="I141">
-        <v>369.48367173206498</v>
-      </c>
-      <c r="J141">
-        <v>11593591.823872698</v>
-      </c>
-    </row>
-    <row r="142" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="I142">
-        <v>372.00063895769102</v>
-      </c>
-      <c r="J142">
-        <v>11659547.034409301</v>
-      </c>
-    </row>
-    <row r="143" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="I143">
-        <v>374.59520054865499</v>
-      </c>
-      <c r="J143">
-        <v>11734352.852242298</v>
-      </c>
-    </row>
-    <row r="144" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="I144">
-        <v>377.37317444714603</v>
-      </c>
-      <c r="J144">
-        <v>11814713.841294598</v>
-      </c>
-    </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I145">
-        <v>379.281987237473</v>
-      </c>
-      <c r="J145">
-        <v>11875887.7407736</v>
-      </c>
-    </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I146">
-        <v>381.434535269874</v>
-      </c>
-      <c r="J146">
-        <v>11937156.090984702</v>
-      </c>
-    </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I147">
-        <v>383.56368688996298</v>
-      </c>
-      <c r="J147">
-        <v>11957858.4496883</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33136,7 +33329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0737387E-079F-42FD-BAAB-95AC0AD4E1E7}">
   <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Fixed Sizing Code, begun final report
</commit_message>
<xml_diff>
--- a/MAE 159/Other data/159 Digitized Plots.xlsx
+++ b/MAE 159/Other data/159 Digitized Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy Slagle\Documents\MAE136-MAE158-MAE159_Aircraft_Design_and_Analysis_Course_Series\MAE 159\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C6CA92-0F83-461F-B2B5-B697132B22F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0E0822-40F4-4724-8260-B9C8FF2BEA2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 1a" sheetId="6" r:id="rId1"/>
@@ -14607,10 +14607,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>60375</c:v>
+                  <c:v>54375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60375</c:v>
+                  <c:v>54375</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>51375</c:v>
@@ -21203,7 +21203,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21488,7 +21488,8 @@
         <v>72</v>
       </c>
       <c r="C21">
-        <v>60375</v>
+        <f>H25</f>
+        <v>54375</v>
       </c>
       <c r="D21">
         <f>H24</f>
@@ -21533,11 +21534,11 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <f>C23</f>
-        <v>60375</v>
+        <v>54375</v>
       </c>
       <c r="C23">
         <f>C21</f>
-        <v>60375</v>
+        <v>54375</v>
       </c>
       <c r="D23">
         <f>D21</f>

</xml_diff>